<commit_message>
updated interface and controllers
</commit_message>
<xml_diff>
--- a/EPICDocuments/burndownchart.xlsx
+++ b/EPICDocuments/burndownchart.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="374" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="374" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -907,11 +908,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="294137264"/>
-        <c:axId val="294134128"/>
+        <c:axId val="281930144"/>
+        <c:axId val="281944744"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="294137264"/>
+        <c:axId val="281930144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -929,7 +930,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="294134128"/>
+        <c:crossAx val="281944744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -937,7 +938,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="294134128"/>
+        <c:axId val="281944744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -986,7 +987,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="294137264"/>
+        <c:crossAx val="281930144"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1213,55 +1214,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>444</c:v>
+                  <c:v>389</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>426.2</c:v>
+                  <c:v>373.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>408.5</c:v>
+                  <c:v>357.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>390.7</c:v>
+                  <c:v>342.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>380.5</c:v>
+                  <c:v>331.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>385.6</c:v>
+                  <c:v>369.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>366.3</c:v>
+                  <c:v>351.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>347</c:v>
+                  <c:v>332.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>327.8</c:v>
+                  <c:v>314.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>308.5</c:v>
+                  <c:v>295.7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>294.60000000000002</c:v>
+                  <c:v>290.39999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>275</c:v>
+                  <c:v>271</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>278.7</c:v>
+                  <c:v>272</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>257.3</c:v>
+                  <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>254.8</c:v>
+                  <c:v>253.4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>234.4</c:v>
+                  <c:v>232.8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>213.1</c:v>
+                  <c:v>210.6</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>200.6</c:v>
@@ -1412,52 +1413,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>444</c:v>
+                  <c:v>389</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>402</c:v>
+                  <c:v>347</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>333</c:v>
+                  <c:v>278</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>313</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>336</c:v>
+                  <c:v>316</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>326</c:v>
+                  <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>320</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>318</c:v>
+                  <c:v>298</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>313</c:v>
+                  <c:v>293</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>294</c:v>
+                  <c:v>287</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>267</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>284</c:v>
+                  <c:v>271</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>225</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>245</c:v>
+                  <c:v>242</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>227</c:v>
+                  <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>205</c:v>
+                  <c:v>198</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>176</c:v>
@@ -1488,8 +1489,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="296186704"/>
-        <c:axId val="296187096"/>
+        <c:axId val="281593504"/>
+        <c:axId val="281592720"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1576,7 +1577,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="296186704"/>
+        <c:axId val="281593504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1675,7 +1676,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="296187096"/>
+        <c:crossAx val="281592720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1683,7 +1684,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="296187096"/>
+        <c:axId val="281592720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,7 +1694,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="296186704"/>
+        <c:crossAx val="281593504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2313,7 +2314,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="75" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2359,7 +2360,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9309919" cy="6083710"/>
+    <xdr:ext cx="9296400" cy="6070600"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3491,8 +3492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3525,71 +3526,71 @@
       <c r="D1" s="41"/>
       <c r="E1" s="8">
         <f>F4</f>
-        <v>444</v>
+        <v>389</v>
       </c>
       <c r="F1" s="8">
         <f>ROUND(F4*(1-1/25),1)</f>
-        <v>426.2</v>
+        <v>373.4</v>
       </c>
       <c r="G1" s="8">
         <f>ROUND(G4*(1-2/25),1)</f>
-        <v>408.5</v>
+        <v>357.9</v>
       </c>
       <c r="H1" s="8">
         <f>ROUND(H4*(1-3/25),1)</f>
-        <v>390.7</v>
+        <v>342.3</v>
       </c>
       <c r="I1" s="8">
         <f>ROUND(I4*(1-4/25),1)</f>
-        <v>380.5</v>
+        <v>331.8</v>
       </c>
       <c r="J1" s="8">
         <f>ROUND(J4*(1-5/25),1)</f>
-        <v>385.6</v>
+        <v>369.6</v>
       </c>
       <c r="K1" s="8">
         <f>ROUND(K4*(1-6/25),1)</f>
-        <v>366.3</v>
+        <v>351.1</v>
       </c>
       <c r="L1" s="8">
         <f>ROUND(L4*(1-7/25),1)</f>
-        <v>347</v>
+        <v>332.6</v>
       </c>
       <c r="M1" s="8">
         <f>ROUND(M4*(1-8/25),1)</f>
-        <v>327.8</v>
+        <v>314.2</v>
       </c>
       <c r="N1" s="8">
         <f>ROUND(N4*(1-9/25),1)</f>
-        <v>308.5</v>
+        <v>295.7</v>
       </c>
       <c r="O1" s="8">
         <f>ROUND(O4*(1-10/25),1)</f>
-        <v>294.60000000000002</v>
+        <v>290.39999999999998</v>
       </c>
       <c r="P1" s="8">
         <f>ROUND(P4*(1-11/25),1)</f>
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="Q1" s="8">
         <f>ROUND(Q4*(1-12/25),1)</f>
-        <v>278.7</v>
+        <v>272</v>
       </c>
       <c r="R1" s="8">
         <f>ROUND(R4*(1-13/25),1)</f>
-        <v>257.3</v>
+        <v>251</v>
       </c>
       <c r="S1" s="8">
         <f>ROUND(S4*(1-14/25),1)</f>
-        <v>254.8</v>
+        <v>253.4</v>
       </c>
       <c r="T1" s="8">
         <f>ROUND(T4*(1-15/25),1)</f>
-        <v>234.4</v>
+        <v>232.8</v>
       </c>
       <c r="U1" s="8">
         <f>ROUND(U4*(1-16/25),1)</f>
-        <v>213.1</v>
+        <v>210.6</v>
       </c>
       <c r="V1" s="8">
         <f>ROUND(V4*(1-17/25),1)</f>
@@ -3746,67 +3747,67 @@
       <c r="E3" s="11"/>
       <c r="F3" s="8">
         <f>F4</f>
-        <v>444</v>
+        <v>389</v>
       </c>
       <c r="G3" s="8">
         <f>G4-F2</f>
-        <v>402</v>
+        <v>347</v>
       </c>
       <c r="H3" s="8">
         <f>H4-G2</f>
-        <v>333</v>
+        <v>278</v>
       </c>
       <c r="I3" s="8">
-        <f t="shared" ref="I3:AA3" si="1">I4-H2</f>
-        <v>313</v>
+        <f t="shared" ref="I3:Z3" si="1">I4-H2</f>
+        <v>255</v>
       </c>
       <c r="J3" s="8">
         <f t="shared" si="1"/>
-        <v>336</v>
+        <v>316</v>
       </c>
       <c r="K3" s="8">
         <f t="shared" si="1"/>
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="L3" s="8">
         <f t="shared" si="1"/>
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="M3" s="8">
         <f t="shared" si="1"/>
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="N3" s="8">
         <f t="shared" si="1"/>
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="O3" s="8">
         <f t="shared" si="1"/>
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="P3" s="8">
         <f t="shared" si="1"/>
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="Q3" s="8">
         <f t="shared" si="1"/>
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="R3" s="8">
         <f t="shared" si="1"/>
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="S3" s="8">
         <f t="shared" si="1"/>
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="T3" s="8">
         <f t="shared" si="1"/>
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="U3" s="8">
         <f t="shared" si="1"/>
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="V3" s="8">
         <f t="shared" si="1"/>
@@ -3839,67 +3840,67 @@
       <c r="E4" s="11"/>
       <c r="F4" s="8">
         <f>SUM($E7:$E14,$E18,$E20:$E32,$E39,$E43:$E44,$E47:$E48,$E56:$E57,$E54,$E59:$E66,$E68:$E69,$E71:$E79)</f>
-        <v>444</v>
+        <v>389</v>
       </c>
       <c r="G4" s="8">
         <f>SUM($E7:$E14,$E18,$E20:$E32,$E39,$E43:$E44,$E47:$E48,$E56:$E57,$E54,$E59:$E66,$E68:$E69,$E71:$E79)</f>
-        <v>444</v>
+        <v>389</v>
       </c>
       <c r="H4" s="8">
         <f>SUM($E7:$E14,$E18,$E20:$E32,$E39,$E43:$E44,$E47:$E48,$E56:$E57,$E54,$E59:$E66,$E68:$E69,$E71:$E79)</f>
-        <v>444</v>
+        <v>389</v>
       </c>
       <c r="I4" s="8">
         <f>SUM($E7:$E14,$E18,$E20:$E32,$E39,$E43:$E44,$E47:$E48,$E56:$E57,$E54,$E59:$E66,$E68:$E69,$E37,$E71:$E79)</f>
-        <v>453</v>
+        <v>395</v>
       </c>
       <c r="J4" s="8">
         <f>SUM($E45,$E50:$E52,$E58,$E7:$E14,$E18,$E20:$E32,$E39,$E43:$E44,$E47:$E48,$E56:$E57,$E54,$E59:$E66,$E68:$E69,$E37,$E71:$E79)</f>
-        <v>482</v>
+        <v>462</v>
       </c>
       <c r="K4" s="8">
         <f t="shared" ref="K4:N4" si="2">SUM($E45,$E50:$E52,$E58,$E7:$E14,$E18,$E20:$E32,$E39,$E43:$E44,$E47:$E48,$E56:$E57,$E54,$E59:$E66,$E68:$E69,$E37,$E71:$E79)</f>
-        <v>482</v>
+        <v>462</v>
       </c>
       <c r="L4" s="8">
         <f t="shared" si="2"/>
-        <v>482</v>
+        <v>462</v>
       </c>
       <c r="M4" s="8">
         <f t="shared" si="2"/>
-        <v>482</v>
+        <v>462</v>
       </c>
       <c r="N4" s="8">
         <f t="shared" si="2"/>
-        <v>482</v>
+        <v>462</v>
       </c>
       <c r="O4" s="8">
         <f>SUM($E45,$E50:$E52,$E58,$E7:$E14,$E18,$E20:$E32,$E39,$E43:$E44,$E47:$E48,$E56:$E57,$E53,$E54,$E59:$E66,$E68:$E69,$E37,$E71:$E79)</f>
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="P4" s="8">
         <f>SUM($E45,$E50:$E52,$E58,$E7:$E14,$E18,$E20:$E32,$E39,$E43:$E44,$E47:$E48,$E56:$E57,$E53,$E54,$E59:$E66,$E68:$E69,$E37,$E71:$E79)</f>
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="Q4" s="8">
         <f>SUM($E16:E17,$E49,$E67,$E45,$E50:$E52,$E58,$E7:$E14,$E18,$E20:$E32,$E39,$E43:$E44,$E47:$E48,$E56:$E57,$E53,$E54,$E67,$E59:$E66,$E37,$E68:$E69,$E71:$E79)</f>
-        <v>536</v>
+        <v>523</v>
       </c>
       <c r="R4" s="8">
         <f>SUM($E16:F17,$E49,$E67,$E45,$E50:$E52,$E58,$E7:$E14,$E18,$E20:$E32,$E39,$E43:$E44,$E47:$E48,$E56:$E57,$E53,$E54,$E67,$E59:$E66,$E37,$E68:$E69,$E71:$E79)</f>
-        <v>536</v>
+        <v>523</v>
       </c>
       <c r="S4" s="8">
         <f>SUM($E16:G17,$E49,$E67,$E45,$E50:$E52,$E58,$E7:$E14,$E18,$E20:$E32,$E39,$E43:$E44,$E47:$E48,$E56:$E57,$E53,$E54,$E67,$E59:$E66,$E37,$E68:$E69,$E19,$E33,$E38,$E40:$E41,$E70,$E71:$E79)</f>
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="T4" s="8">
         <f>SUM($E16:H17,$E49,$E67,$E45,$E50:$E52,$E58,$E7:$E14,$E18,$E20:$E32,$E39,$E43:$E44,$E47:$E48,$E56:$E57,$E53,$E54,$E67,$E59:$E66,$E37,$E68:$E69,$E19,$E33,$E38,$E40:$E41,$E70,$E42,$E71:$E79)</f>
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="U4" s="8">
         <f>SUM($E16:I17,$E49,$E67,$E45,$E50:$E52,$E58,$E7:$E14,$E18,$E20:$E32,$E39,$E43:$E44,$E47:$E48,$E56:$E57,$E53,$E54,$E67,$E59:$E66,$E37,$E68:$E69,$E19,$E33,$E38,$E40:$E41,$E70,$E15,$E42,$E71:$E79)</f>
-        <v>592</v>
+        <v>585</v>
       </c>
       <c r="V4" s="8">
         <f>SUM(E7:E79)</f>
@@ -4062,7 +4063,7 @@
         <v>42136</v>
       </c>
       <c r="D7" s="17">
-        <f t="shared" ref="D7:D70" si="4">SUM(F7:AD7)</f>
+        <f>SUM(F7:AD7)</f>
         <v>9</v>
       </c>
       <c r="E7" s="19">
@@ -4095,7 +4096,7 @@
         <v>42136</v>
       </c>
       <c r="D8" s="17">
-        <f t="shared" si="4"/>
+        <f>SUM(F8:AD8)</f>
         <v>6</v>
       </c>
       <c r="E8" s="19">
@@ -4122,7 +4123,7 @@
         <v>42136</v>
       </c>
       <c r="D9" s="17">
-        <f t="shared" si="4"/>
+        <f>SUM(F9:AD9)</f>
         <v>7</v>
       </c>
       <c r="E9" s="19">
@@ -4155,7 +4156,7 @@
         <v>42136</v>
       </c>
       <c r="D10" s="17">
-        <f t="shared" si="4"/>
+        <f>SUM(F10:AD10)</f>
         <v>9</v>
       </c>
       <c r="E10" s="19">
@@ -4194,7 +4195,7 @@
         <v>42136</v>
       </c>
       <c r="D11" s="17">
-        <f t="shared" si="4"/>
+        <f>SUM(F11:AD11)</f>
         <v>5</v>
       </c>
       <c r="E11" s="19">
@@ -4221,7 +4222,7 @@
         <v>42136</v>
       </c>
       <c r="D12" s="17">
-        <f t="shared" si="4"/>
+        <f>SUM(F12:AD12)</f>
         <v>4</v>
       </c>
       <c r="E12" s="19">
@@ -4245,7 +4246,7 @@
         <v>42136</v>
       </c>
       <c r="D13" s="17">
-        <f t="shared" si="4"/>
+        <f>SUM(F13:AD13)</f>
         <v>4</v>
       </c>
       <c r="E13" s="19">
@@ -4269,7 +4270,7 @@
         <v>42136</v>
       </c>
       <c r="D14" s="17">
-        <f t="shared" si="4"/>
+        <f>SUM(F14:AD14)</f>
         <v>4</v>
       </c>
       <c r="E14" s="19">
@@ -4280,1602 +4281,2538 @@
       </c>
     </row>
     <row r="15" spans="1:30" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="33">
-        <v>42237</v>
-      </c>
-      <c r="D15" s="32">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="E15" s="34">
-        <v>6</v>
-      </c>
-      <c r="T15" s="32">
+      <c r="A15" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D15" s="17">
+        <f>SUM(F15:AD15)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="19">
+        <v>3</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="17"/>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="17"/>
+    </row>
+    <row r="16" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D16" s="17">
+        <f>SUM(F16:AD16)</f>
+        <v>8</v>
+      </c>
+      <c r="E16" s="19">
+        <v>9</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17">
+        <v>5</v>
+      </c>
+      <c r="R16" s="17">
+        <v>1</v>
+      </c>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17">
+        <v>1</v>
+      </c>
+      <c r="U16" s="17">
+        <v>1</v>
+      </c>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="17"/>
+      <c r="AB16" s="17"/>
+      <c r="AC16" s="17"/>
+      <c r="AD16" s="17"/>
+    </row>
+    <row r="17" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D17" s="17">
+        <f>SUM(F17:AD17)</f>
         <v>2</v>
       </c>
-      <c r="U15" s="32">
+      <c r="E17" s="19">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" s="24">
-        <v>42209</v>
-      </c>
-      <c r="D16" s="23">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="E16" s="25">
-        <v>10</v>
-      </c>
-      <c r="Q16" s="23">
-        <v>5</v>
-      </c>
-      <c r="U16" s="23">
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="17"/>
+      <c r="Y17" s="17">
         <v>2</v>
       </c>
-      <c r="X16" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="C17" s="24">
-        <v>42209</v>
-      </c>
-      <c r="D17" s="23">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="E17" s="25">
-        <v>5</v>
-      </c>
-      <c r="Q17" s="23">
-        <v>2</v>
-      </c>
-      <c r="U17" s="23">
-        <v>2</v>
-      </c>
-      <c r="X17" s="23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z17" s="17"/>
+      <c r="AA17" s="17"/>
+      <c r="AB17" s="17"/>
+      <c r="AC17" s="17"/>
+      <c r="AD17" s="17"/>
+    </row>
+    <row r="18" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C18" s="18">
         <v>42136</v>
       </c>
       <c r="D18" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>SUM(F18:AD18)</f>
+        <v>3</v>
       </c>
       <c r="E18" s="19">
+        <v>5</v>
+      </c>
+      <c r="Y18" s="17">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:25" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="C19" s="36">
-        <v>42224</v>
-      </c>
-      <c r="D19" s="35">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="37">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" s="17" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D19" s="17">
+        <f>SUM(F19:AD19)</f>
+        <v>9</v>
+      </c>
+      <c r="E19" s="19">
+        <v>7</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="17">
+        <v>3</v>
+      </c>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17">
+        <v>4</v>
+      </c>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="17"/>
+      <c r="AA19" s="17"/>
+      <c r="AB19" s="17"/>
+      <c r="AC19" s="17"/>
+      <c r="AD19" s="17"/>
+    </row>
+    <row r="20" spans="1:30" s="17" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C20" s="18">
         <v>42136</v>
       </c>
       <c r="D20" s="17">
-        <f t="shared" si="4"/>
-        <v>8</v>
+        <f>SUM(F20:AD20)</f>
+        <v>6</v>
       </c>
       <c r="E20" s="19">
-        <v>9</v>
-      </c>
-      <c r="Q20" s="17">
-        <v>5</v>
-      </c>
-      <c r="R20" s="17">
-        <v>1</v>
-      </c>
-      <c r="T20" s="17">
-        <v>1</v>
-      </c>
-      <c r="U20" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F20" s="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C21" s="18">
         <v>42136</v>
       </c>
       <c r="D21" s="17">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <f>SUM(F21:AD21)</f>
+        <v>4</v>
       </c>
       <c r="E21" s="19">
-        <v>5</v>
-      </c>
-      <c r="Y21" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F21" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C22" s="18">
         <v>42136</v>
       </c>
       <c r="D22" s="17">
-        <f t="shared" si="4"/>
+        <f>SUM(F22:AD22)</f>
         <v>3</v>
       </c>
       <c r="E22" s="19">
         <v>5</v>
       </c>
-      <c r="Y22" s="17">
+      <c r="G22" s="17">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C23" s="18">
         <v>42136</v>
       </c>
       <c r="D23" s="17">
-        <f t="shared" si="4"/>
-        <v>9</v>
+        <f>SUM(F23:AD23)</f>
+        <v>3</v>
       </c>
       <c r="E23" s="19">
-        <v>7</v>
-      </c>
-      <c r="P23" s="17">
-        <v>2</v>
-      </c>
-      <c r="Q23" s="17">
+        <v>4</v>
+      </c>
+      <c r="G23" s="17">
         <v>3</v>
       </c>
-      <c r="U23" s="17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C24" s="18">
         <v>42136</v>
       </c>
       <c r="D24" s="17">
-        <f t="shared" si="4"/>
-        <v>6</v>
+        <f>SUM(F24:AD24)</f>
+        <v>8</v>
       </c>
       <c r="E24" s="19">
-        <v>6</v>
-      </c>
-      <c r="F24" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G24" s="17">
+        <v>1</v>
+      </c>
+      <c r="H24" s="17">
+        <v>0</v>
+      </c>
+      <c r="I24" s="17">
+        <v>1</v>
+      </c>
+      <c r="J24" s="17">
+        <v>1</v>
+      </c>
+      <c r="K24" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C25" s="18">
         <v>42136</v>
       </c>
       <c r="D25" s="17">
-        <f t="shared" si="4"/>
+        <f>SUM(F25:AD25)</f>
+        <v>13</v>
+      </c>
+      <c r="E25" s="19">
+        <v>12</v>
+      </c>
+      <c r="G25" s="17">
+        <v>5</v>
+      </c>
+      <c r="I25" s="17">
         <v>4</v>
       </c>
-      <c r="E25" s="19">
-        <v>6</v>
-      </c>
-      <c r="F25" s="17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="17">
+        <v>2</v>
+      </c>
+      <c r="L25" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C26" s="18">
         <v>42136</v>
       </c>
       <c r="D26" s="17">
-        <f t="shared" si="4"/>
+        <f>SUM(F26:AD26)</f>
+        <v>12</v>
+      </c>
+      <c r="E26" s="19">
+        <v>10</v>
+      </c>
+      <c r="G26" s="17">
+        <v>2</v>
+      </c>
+      <c r="P26" s="17">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="17">
         <v>3</v>
       </c>
-      <c r="E26" s="19">
+      <c r="U26" s="17">
         <v>5</v>
       </c>
-      <c r="G26" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C27" s="18">
         <v>42136</v>
       </c>
       <c r="D27" s="17">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <f>SUM(F27:AD27)</f>
+        <v>10</v>
       </c>
       <c r="E27" s="19">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G27" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="H27" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C28" s="18">
         <v>42136</v>
       </c>
       <c r="D28" s="17">
-        <f t="shared" si="4"/>
-        <v>8</v>
+        <f>SUM(F28:AD28)</f>
+        <v>11</v>
       </c>
       <c r="E28" s="19">
+        <v>10</v>
+      </c>
+      <c r="H28" s="17">
+        <v>1</v>
+      </c>
+      <c r="I28" s="17">
+        <v>1</v>
+      </c>
+      <c r="M28" s="17">
         <v>5</v>
       </c>
-      <c r="G28" s="17">
-        <v>1</v>
-      </c>
-      <c r="H28" s="17">
-        <v>0</v>
-      </c>
-      <c r="I28" s="17">
-        <v>1</v>
-      </c>
-      <c r="J28" s="17">
-        <v>1</v>
-      </c>
-      <c r="K28" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N28" s="17">
+        <v>2</v>
+      </c>
+      <c r="R28" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="C29" s="18">
         <v>42136</v>
       </c>
       <c r="D29" s="17">
-        <f t="shared" si="4"/>
-        <v>13</v>
+        <f>SUM(F29:AD29)</f>
+        <v>5</v>
       </c>
       <c r="E29" s="19">
-        <v>12</v>
-      </c>
-      <c r="G29" s="17">
+        <v>2</v>
+      </c>
+      <c r="W29" s="17">
         <v>5</v>
       </c>
-      <c r="I29" s="17">
-        <v>4</v>
-      </c>
-      <c r="J29" s="17">
-        <v>2</v>
-      </c>
-      <c r="L29" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>4</v>
+        <v>125</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="C30" s="18">
         <v>42136</v>
       </c>
       <c r="D30" s="17">
-        <f t="shared" si="4"/>
-        <v>12</v>
+        <f>SUM(F30:AD30)</f>
+        <v>11</v>
       </c>
       <c r="E30" s="19">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="F30" s="17">
+        <v>3</v>
       </c>
       <c r="G30" s="17">
         <v>2</v>
       </c>
-      <c r="P30" s="17">
+      <c r="N30" s="17">
+        <v>4</v>
+      </c>
+      <c r="O30" s="17">
         <v>2</v>
       </c>
-      <c r="Q30" s="17">
-        <v>3</v>
-      </c>
-      <c r="U30" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>4</v>
+        <v>125</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="C31" s="18">
         <v>42136</v>
       </c>
       <c r="D31" s="17">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f>SUM(F31:AD31)</f>
+        <v>11</v>
       </c>
       <c r="E31" s="19">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G31" s="17">
-        <v>5</v>
-      </c>
-      <c r="H31" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="P31" s="17">
+        <v>6</v>
+      </c>
+      <c r="Q31" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>4</v>
+        <v>125</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>115</v>
+        <v>35</v>
       </c>
       <c r="C32" s="18">
         <v>42136</v>
       </c>
       <c r="D32" s="17">
-        <f t="shared" si="4"/>
-        <v>11</v>
+        <f>SUM(F32:AD32)</f>
+        <v>9</v>
       </c>
       <c r="E32" s="19">
-        <v>10</v>
-      </c>
-      <c r="H32" s="17">
-        <v>1</v>
-      </c>
-      <c r="I32" s="17">
-        <v>1</v>
-      </c>
-      <c r="M32" s="17">
+        <v>9</v>
+      </c>
+      <c r="O32" s="17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D33" s="17">
+        <f>SUM(F33:AD33)</f>
+        <v>9</v>
+      </c>
+      <c r="E33" s="19">
+        <v>8</v>
+      </c>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17">
+        <v>9</v>
+      </c>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="17"/>
+      <c r="V33" s="17"/>
+      <c r="W33" s="17"/>
+      <c r="X33" s="17"/>
+      <c r="Y33" s="17"/>
+      <c r="Z33" s="17"/>
+      <c r="AA33" s="17"/>
+      <c r="AB33" s="17"/>
+      <c r="AC33" s="17"/>
+      <c r="AD33" s="17"/>
+    </row>
+    <row r="34" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D34" s="17">
+        <f>SUM(F34:AD34)</f>
+        <v>12</v>
+      </c>
+      <c r="E34" s="19">
+        <v>12</v>
+      </c>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17">
+        <v>2</v>
+      </c>
+      <c r="Q34" s="17">
         <v>5</v>
       </c>
-      <c r="N32" s="17">
-        <v>2</v>
-      </c>
-      <c r="R32" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="C33" s="36">
-        <v>42223</v>
-      </c>
-      <c r="D33" s="35">
-        <f t="shared" si="4"/>
+      <c r="R34" s="17">
         <v>5</v>
       </c>
-      <c r="E33" s="37">
-        <v>5</v>
-      </c>
-      <c r="W33" s="35">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="C34" s="39">
-        <v>42251</v>
-      </c>
-      <c r="D34" s="38">
-        <f t="shared" si="4"/>
+      <c r="S34" s="17"/>
+      <c r="T34" s="17"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="17"/>
+      <c r="Y34" s="17"/>
+      <c r="Z34" s="17"/>
+      <c r="AA34" s="17"/>
+      <c r="AB34" s="17"/>
+      <c r="AC34" s="17"/>
+      <c r="AD34" s="17"/>
+    </row>
+    <row r="35" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D35" s="17">
+        <f>SUM(F35:AD35)</f>
         <v>0</v>
       </c>
-      <c r="E34" s="40">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="C35" s="39">
-        <v>42251</v>
-      </c>
-      <c r="D35" s="38">
-        <f t="shared" si="4"/>
+      <c r="E35" s="19">
+        <v>6</v>
+      </c>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="17"/>
+      <c r="R35" s="17"/>
+      <c r="S35" s="17"/>
+      <c r="T35" s="17"/>
+      <c r="U35" s="17"/>
+      <c r="V35" s="17"/>
+      <c r="W35" s="17"/>
+      <c r="X35" s="17"/>
+      <c r="Y35" s="17"/>
+      <c r="Z35" s="17"/>
+      <c r="AA35" s="17"/>
+      <c r="AB35" s="17"/>
+      <c r="AC35" s="17"/>
+      <c r="AD35" s="17"/>
+    </row>
+    <row r="36" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D36" s="17">
+        <f>SUM(F36:AD36)</f>
         <v>0</v>
       </c>
-      <c r="E35" s="40">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="C36" s="39">
-        <v>42251</v>
-      </c>
-      <c r="D36" s="38">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="E36" s="40">
+      <c r="E36" s="19">
         <v>6</v>
       </c>
-      <c r="S36" s="38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="17"/>
+      <c r="Q36" s="17"/>
+      <c r="R36" s="17"/>
+      <c r="S36" s="17"/>
+      <c r="T36" s="17"/>
+      <c r="U36" s="17"/>
+      <c r="V36" s="17"/>
+      <c r="W36" s="17"/>
+      <c r="X36" s="17"/>
+      <c r="Y36" s="17"/>
+      <c r="Z36" s="17"/>
+      <c r="AA36" s="17"/>
+      <c r="AB36" s="17"/>
+      <c r="AC36" s="17"/>
+      <c r="AD36" s="17"/>
+    </row>
+    <row r="37" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>4</v>
+        <v>125</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="C37" s="18">
-        <v>42153</v>
+        <v>42136</v>
       </c>
       <c r="D37" s="17">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f>SUM(F37:AD37)</f>
+        <v>0</v>
       </c>
       <c r="E37" s="19">
-        <v>9</v>
-      </c>
-      <c r="N37" s="17">
-        <v>2</v>
-      </c>
-      <c r="O37" s="17">
-        <v>3</v>
-      </c>
-      <c r="T37" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="35" t="s">
-        <v>121</v>
-      </c>
-      <c r="C38" s="36">
-        <v>42223</v>
-      </c>
-      <c r="D38" s="35">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="E38" s="37">
-        <v>9</v>
-      </c>
-      <c r="W38" s="35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D38" s="17">
+        <f>SUM(F38:AD38)</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="19">
+        <v>13</v>
+      </c>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="17"/>
+      <c r="Q38" s="17"/>
+      <c r="R38" s="17"/>
+      <c r="S38" s="17"/>
+      <c r="T38" s="17"/>
+      <c r="U38" s="17"/>
+      <c r="V38" s="17"/>
+      <c r="W38" s="17"/>
+      <c r="X38" s="17"/>
+      <c r="Y38" s="17"/>
+      <c r="Z38" s="17"/>
+      <c r="AA38" s="17"/>
+      <c r="AB38" s="17"/>
+      <c r="AC38" s="17"/>
+      <c r="AD38" s="17"/>
+    </row>
+    <row r="39" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C39" s="18">
         <v>42136</v>
       </c>
       <c r="D39" s="17">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f>SUM(F39:AD39)</f>
+        <v>9</v>
       </c>
       <c r="E39" s="19">
-        <v>2</v>
-      </c>
-      <c r="W39" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="17">
+        <v>3</v>
+      </c>
+      <c r="G39" s="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D40" s="17">
+        <f>SUM(F40:AD40)</f>
+        <v>3</v>
+      </c>
+      <c r="E40" s="19">
+        <v>13</v>
+      </c>
+      <c r="F40" s="17">
+        <v>3</v>
+      </c>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="17"/>
+      <c r="O40" s="17"/>
+      <c r="P40" s="17"/>
+      <c r="Q40" s="17"/>
+      <c r="R40" s="17"/>
+      <c r="S40" s="17"/>
+      <c r="T40" s="17"/>
+      <c r="U40" s="17"/>
+      <c r="V40" s="17"/>
+      <c r="W40" s="17"/>
+      <c r="X40" s="17"/>
+      <c r="Y40" s="17"/>
+      <c r="Z40" s="17"/>
+      <c r="AA40" s="17"/>
+      <c r="AB40" s="17"/>
+      <c r="AC40" s="17"/>
+      <c r="AD40" s="17"/>
+    </row>
+    <row r="41" spans="1:30" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D41" s="17">
+        <f>SUM(F41:AD41)</f>
         <v>4</v>
       </c>
-      <c r="B40" s="35" t="s">
-        <v>123</v>
-      </c>
-      <c r="C40" s="36">
-        <v>42223</v>
-      </c>
-      <c r="D40" s="35">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="E40" s="37">
-        <v>5</v>
-      </c>
-      <c r="T40" s="35">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C41" s="36">
-        <v>42223</v>
-      </c>
-      <c r="D41" s="35">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="E41" s="37">
-        <v>4</v>
-      </c>
-      <c r="N41" s="35">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="C42" s="30">
-        <v>42230</v>
-      </c>
-      <c r="D42" s="29">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="E42" s="31">
-        <v>7</v>
-      </c>
-      <c r="T42" s="29">
-        <v>2</v>
-      </c>
-      <c r="U42" s="29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E41" s="19">
+        <v>8</v>
+      </c>
+      <c r="F41" s="17">
+        <v>3</v>
+      </c>
+      <c r="G41" s="17">
+        <v>1</v>
+      </c>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="17"/>
+      <c r="Q41" s="17"/>
+      <c r="R41" s="17"/>
+      <c r="S41" s="17"/>
+      <c r="T41" s="17"/>
+      <c r="U41" s="17"/>
+      <c r="V41" s="17"/>
+      <c r="W41" s="17"/>
+      <c r="X41" s="17"/>
+      <c r="Y41" s="17"/>
+      <c r="Z41" s="17"/>
+      <c r="AA41" s="17"/>
+      <c r="AB41" s="17"/>
+      <c r="AC41" s="17"/>
+      <c r="AD41" s="17"/>
+    </row>
+    <row r="42" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C42" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D42" s="17">
+        <f>SUM(F42:AD42)</f>
+        <v>3</v>
+      </c>
+      <c r="E42" s="19">
+        <v>6</v>
+      </c>
+      <c r="F42" s="17">
+        <v>3</v>
+      </c>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="17"/>
+      <c r="R42" s="17"/>
+      <c r="S42" s="17"/>
+      <c r="T42" s="17"/>
+      <c r="U42" s="17"/>
+      <c r="V42" s="17"/>
+      <c r="W42" s="17"/>
+      <c r="X42" s="17"/>
+      <c r="Y42" s="17"/>
+      <c r="Z42" s="17"/>
+      <c r="AA42" s="17"/>
+      <c r="AB42" s="17"/>
+      <c r="AC42" s="17"/>
+      <c r="AD42" s="17"/>
+    </row>
+    <row r="43" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>125</v>
+        <v>6</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C43" s="18">
         <v>42136</v>
       </c>
       <c r="D43" s="17">
-        <f t="shared" si="4"/>
-        <v>11</v>
+        <f>SUM(F43:AD43)</f>
+        <v>4</v>
       </c>
       <c r="E43" s="19">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F43" s="17">
         <v>3</v>
       </c>
       <c r="G43" s="17">
-        <v>2</v>
-      </c>
-      <c r="N43" s="17">
-        <v>4</v>
-      </c>
-      <c r="O43" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>125</v>
+        <v>6</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="C44" s="18">
         <v>42136</v>
       </c>
       <c r="D44" s="17">
-        <f t="shared" si="4"/>
+        <f>SUM(F44:AD44)</f>
+        <v>4</v>
+      </c>
+      <c r="E44" s="19">
+        <v>8</v>
+      </c>
+      <c r="F44" s="17">
+        <v>3</v>
+      </c>
+      <c r="G44" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D45" s="17">
+        <f>SUM(F45:AD45)</f>
         <v>11</v>
       </c>
-      <c r="E44" s="19">
+      <c r="E45" s="19">
         <v>12</v>
       </c>
-      <c r="G44" s="17">
-        <v>4</v>
-      </c>
-      <c r="P44" s="17">
+      <c r="F45" s="17"/>
+      <c r="G45" s="17">
+        <v>1</v>
+      </c>
+      <c r="H45" s="17">
+        <v>2</v>
+      </c>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17">
+        <v>7</v>
+      </c>
+      <c r="K45" s="17">
+        <v>1</v>
+      </c>
+      <c r="L45" s="17"/>
+      <c r="M45" s="17"/>
+      <c r="N45" s="17"/>
+      <c r="O45" s="17"/>
+      <c r="P45" s="17"/>
+      <c r="Q45" s="17"/>
+      <c r="R45" s="17"/>
+      <c r="S45" s="17"/>
+      <c r="T45" s="17"/>
+      <c r="U45" s="17"/>
+      <c r="V45" s="17"/>
+      <c r="W45" s="17"/>
+      <c r="X45" s="17"/>
+      <c r="Y45" s="17"/>
+      <c r="Z45" s="17"/>
+      <c r="AA45" s="17"/>
+      <c r="AB45" s="17"/>
+      <c r="AC45" s="17"/>
+      <c r="AD45" s="17"/>
+    </row>
+    <row r="46" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="Q44" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="B45" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="C45" s="27">
-        <v>42160</v>
-      </c>
-      <c r="D45" s="26">
-        <f t="shared" si="4"/>
+      <c r="B46" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C46" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D46" s="17">
+        <f>SUM(F46:AD46)</f>
+        <v>9</v>
+      </c>
+      <c r="E46" s="19">
+        <v>11</v>
+      </c>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="17">
+        <v>8</v>
+      </c>
+      <c r="O46" s="17">
+        <v>1</v>
+      </c>
+      <c r="P46" s="17"/>
+      <c r="Q46" s="17"/>
+      <c r="R46" s="17"/>
+      <c r="S46" s="17"/>
+      <c r="T46" s="17"/>
+      <c r="U46" s="17"/>
+      <c r="V46" s="17"/>
+      <c r="W46" s="17"/>
+      <c r="X46" s="17"/>
+      <c r="Y46" s="17"/>
+      <c r="Z46" s="17"/>
+      <c r="AA46" s="17"/>
+      <c r="AB46" s="17"/>
+      <c r="AC46" s="17"/>
+      <c r="AD46" s="17"/>
+    </row>
+    <row r="47" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E45" s="28">
-        <v>5</v>
-      </c>
-      <c r="G45" s="26">
-        <v>1</v>
-      </c>
-      <c r="H45" s="26">
-        <v>2</v>
-      </c>
-      <c r="Q45" s="26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="B46" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="C46" s="39">
-        <v>42251</v>
-      </c>
-      <c r="D46" s="38">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="E46" s="40">
-        <v>7</v>
-      </c>
-      <c r="S46" s="38">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
-        <v>125</v>
-      </c>
       <c r="B47" s="17" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C47" s="18">
         <v>42136</v>
       </c>
       <c r="D47" s="17">
-        <f t="shared" si="4"/>
-        <v>9</v>
+        <f>SUM(F47:AD47)</f>
+        <v>0</v>
       </c>
       <c r="E47" s="19">
-        <v>9</v>
-      </c>
-      <c r="O47" s="17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>125</v>
+        <v>6</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="C48" s="18">
         <v>42136</v>
       </c>
       <c r="D48" s="17">
-        <f t="shared" si="4"/>
-        <v>9</v>
+        <f>SUM(F48:AD48)</f>
+        <v>6</v>
       </c>
       <c r="E48" s="19">
-        <v>8</v>
-      </c>
-      <c r="O48" s="17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="B49" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" s="24">
-        <v>42209</v>
-      </c>
-      <c r="D49" s="23">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="E49" s="25">
-        <v>10</v>
-      </c>
-      <c r="G49" s="23">
-        <v>1</v>
-      </c>
-      <c r="S49" s="23">
+        <v>12</v>
+      </c>
+      <c r="F48" s="17">
+        <v>3</v>
+      </c>
+      <c r="G48" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D49" s="17">
+        <f>SUM(F49:AD49)</f>
+        <v>23</v>
+      </c>
+      <c r="E49" s="19">
+        <v>15</v>
+      </c>
+      <c r="F49" s="17">
         <v>7</v>
       </c>
-      <c r="T49" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="B50" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="C50" s="27">
-        <v>42160</v>
-      </c>
-      <c r="D50" s="26">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="E50" s="28">
-        <v>9</v>
-      </c>
-      <c r="G50" s="26">
+      <c r="G49" s="17">
         <v>7</v>
       </c>
-      <c r="H50" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="B51" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="C51" s="27">
-        <v>42160</v>
-      </c>
-      <c r="D51" s="26">
-        <f t="shared" si="4"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="17"/>
+      <c r="M49" s="17"/>
+      <c r="N49" s="17">
+        <v>7</v>
+      </c>
+      <c r="O49" s="17"/>
+      <c r="P49" s="17"/>
+      <c r="Q49" s="17">
+        <v>2</v>
+      </c>
+      <c r="R49" s="17"/>
+      <c r="S49" s="17"/>
+      <c r="T49" s="17"/>
+      <c r="U49" s="17"/>
+      <c r="V49" s="17"/>
+      <c r="W49" s="17"/>
+      <c r="X49" s="17"/>
+      <c r="Y49" s="17"/>
+      <c r="Z49" s="17"/>
+      <c r="AA49" s="17"/>
+      <c r="AB49" s="17"/>
+      <c r="AC49" s="17"/>
+      <c r="AD49" s="17"/>
+    </row>
+    <row r="50" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C50" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D50" s="17">
+        <f>SUM(F50:AD50)</f>
+        <v>19</v>
+      </c>
+      <c r="E50" s="19">
+        <v>20</v>
+      </c>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17">
+        <v>3</v>
+      </c>
+      <c r="H50" s="17">
+        <v>2</v>
+      </c>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
+      <c r="Q50" s="17">
         <v>4</v>
       </c>
-      <c r="E51" s="28">
+      <c r="R50" s="17">
+        <v>2</v>
+      </c>
+      <c r="S50" s="17"/>
+      <c r="T50" s="17"/>
+      <c r="U50" s="17">
+        <v>7</v>
+      </c>
+      <c r="V50" s="17"/>
+      <c r="W50" s="17"/>
+      <c r="X50" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y50" s="17"/>
+      <c r="Z50" s="17"/>
+      <c r="AA50" s="17"/>
+      <c r="AB50" s="17"/>
+      <c r="AC50" s="17"/>
+      <c r="AD50" s="17"/>
+    </row>
+    <row r="51" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D51" s="17">
+        <f>SUM(F51:AD51)</f>
+        <v>18</v>
+      </c>
+      <c r="E51" s="19">
+        <v>20</v>
+      </c>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17">
         <v>3</v>
       </c>
-      <c r="P51" s="26">
+      <c r="H51" s="17">
         <v>2</v>
       </c>
-      <c r="Q51" s="26">
+      <c r="I51" s="17"/>
+      <c r="J51" s="17"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="17"/>
+      <c r="O51" s="17"/>
+      <c r="P51" s="17"/>
+      <c r="Q51" s="17">
+        <v>5</v>
+      </c>
+      <c r="R51" s="17"/>
+      <c r="S51" s="17"/>
+      <c r="T51" s="17"/>
+      <c r="U51" s="17">
+        <v>7</v>
+      </c>
+      <c r="V51" s="17"/>
+      <c r="W51" s="17"/>
+      <c r="X51" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y51" s="17"/>
+      <c r="Z51" s="17"/>
+      <c r="AA51" s="17"/>
+      <c r="AB51" s="17"/>
+      <c r="AC51" s="17"/>
+      <c r="AD51" s="17"/>
+    </row>
+    <row r="52" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C52" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D52" s="17">
+        <f>SUM(F52:AD52)</f>
+        <v>11</v>
+      </c>
+      <c r="E52" s="19">
+        <v>6</v>
+      </c>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17">
+        <v>0</v>
+      </c>
+      <c r="I52" s="17"/>
+      <c r="J52" s="17"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="17"/>
+      <c r="M52" s="17"/>
+      <c r="N52" s="17"/>
+      <c r="O52" s="17"/>
+      <c r="P52" s="17"/>
+      <c r="Q52" s="17">
+        <v>1</v>
+      </c>
+      <c r="R52" s="17">
+        <v>4</v>
+      </c>
+      <c r="S52" s="17"/>
+      <c r="T52" s="17"/>
+      <c r="U52" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="B52" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C52" s="27">
-        <v>42160</v>
-      </c>
-      <c r="D52" s="26">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="E52" s="28">
+      <c r="V52" s="17">
         <v>3</v>
       </c>
-      <c r="P52" s="26">
+      <c r="W52" s="17"/>
+      <c r="X52" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y52" s="17"/>
+      <c r="Z52" s="17"/>
+      <c r="AA52" s="17"/>
+      <c r="AB52" s="17"/>
+      <c r="AC52" s="17"/>
+      <c r="AD52" s="17"/>
+    </row>
+    <row r="53" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C53" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D53" s="17">
+        <f>SUM(F53:AD53)</f>
+        <v>19</v>
+      </c>
+      <c r="E53" s="19">
+        <v>22</v>
+      </c>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17">
+        <v>3</v>
+      </c>
+      <c r="H53" s="17">
         <v>2</v>
       </c>
-      <c r="Q52" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="B53" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C53" s="21">
-        <v>42190</v>
-      </c>
-      <c r="D53" s="20">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="E53" s="22">
-        <v>9</v>
-      </c>
-      <c r="T53" s="20">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="17"/>
+      <c r="M53" s="17"/>
+      <c r="N53" s="17"/>
+      <c r="O53" s="17"/>
+      <c r="P53" s="17"/>
+      <c r="Q53" s="17">
+        <v>6</v>
+      </c>
+      <c r="R53" s="17"/>
+      <c r="S53" s="17"/>
+      <c r="T53" s="17"/>
+      <c r="U53" s="17">
+        <v>7</v>
+      </c>
+      <c r="V53" s="17"/>
+      <c r="W53" s="17"/>
+      <c r="X53" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y53" s="17"/>
+      <c r="Z53" s="17"/>
+      <c r="AA53" s="17"/>
+      <c r="AB53" s="17"/>
+      <c r="AC53" s="17"/>
+      <c r="AD53" s="17"/>
+    </row>
+    <row r="54" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
-        <v>125</v>
+        <v>7</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>67</v>
+        <v>149</v>
       </c>
       <c r="C54" s="18">
         <v>42136</v>
       </c>
       <c r="D54" s="17">
-        <f t="shared" si="4"/>
+        <f>SUM(F54:AD54)</f>
+        <v>21</v>
+      </c>
+      <c r="E54" s="19">
+        <v>21</v>
+      </c>
+      <c r="G54" s="17">
+        <v>3</v>
+      </c>
+      <c r="H54" s="17">
+        <v>7</v>
+      </c>
+      <c r="Q54" s="17">
+        <v>3</v>
+      </c>
+      <c r="U54" s="17">
+        <v>7</v>
+      </c>
+      <c r="X54" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:30" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" s="18">
+        <v>42136</v>
+      </c>
+      <c r="D55" s="17">
+        <f>SUM(F55:AD55)</f>
+        <v>10</v>
+      </c>
+      <c r="E55" s="19">
         <v>12</v>
       </c>
-      <c r="E54" s="19">
-        <v>12</v>
-      </c>
-      <c r="P54" s="17">
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17">
+        <v>0</v>
+      </c>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="17"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="17"/>
+      <c r="N55" s="17"/>
+      <c r="O55" s="17"/>
+      <c r="P55" s="17"/>
+      <c r="Q55" s="17"/>
+      <c r="R55" s="17">
+        <v>5</v>
+      </c>
+      <c r="S55" s="17"/>
+      <c r="T55" s="17"/>
+      <c r="U55" s="17">
         <v>2</v>
       </c>
-      <c r="Q54" s="17">
+      <c r="V55" s="17">
+        <v>2</v>
+      </c>
+      <c r="W55" s="17"/>
+      <c r="X55" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y55" s="17"/>
+      <c r="Z55" s="17"/>
+      <c r="AA55" s="17"/>
+      <c r="AB55" s="17"/>
+      <c r="AC55" s="17"/>
+      <c r="AD55" s="17"/>
+    </row>
+    <row r="56" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C56" s="18">
+        <v>42153</v>
+      </c>
+      <c r="D56" s="17">
+        <f>SUM(F56:AD56)</f>
+        <v>10</v>
+      </c>
+      <c r="E56" s="19">
+        <v>9</v>
+      </c>
+      <c r="N56" s="17">
+        <v>2</v>
+      </c>
+      <c r="O56" s="17">
+        <v>3</v>
+      </c>
+      <c r="T56" s="17">
         <v>5</v>
       </c>
-      <c r="R54" s="17">
+    </row>
+    <row r="57" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C57" s="27">
+        <v>42160</v>
+      </c>
+      <c r="D57" s="26">
+        <f>SUM(F57:AD57)</f>
+        <v>6</v>
+      </c>
+      <c r="E57" s="28">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:20" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="B55" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="C55" s="39">
-        <v>42251</v>
-      </c>
-      <c r="D55" s="38">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E55" s="40">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C56" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D56" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E56" s="19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C57" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D57" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E57" s="19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F57" s="26"/>
+      <c r="G57" s="26">
+        <v>1</v>
+      </c>
+      <c r="H57" s="26">
+        <v>2</v>
+      </c>
+      <c r="I57" s="26"/>
+      <c r="J57" s="26"/>
+      <c r="K57" s="26"/>
+      <c r="L57" s="26"/>
+      <c r="M57" s="26"/>
+      <c r="N57" s="26"/>
+      <c r="O57" s="26"/>
+      <c r="P57" s="26"/>
+      <c r="Q57" s="26">
+        <v>3</v>
+      </c>
+      <c r="R57" s="26"/>
+      <c r="S57" s="26"/>
+      <c r="T57" s="26"/>
+      <c r="U57" s="26"/>
+      <c r="V57" s="26"/>
+      <c r="W57" s="26"/>
+      <c r="X57" s="26"/>
+      <c r="Y57" s="26"/>
+      <c r="Z57" s="26"/>
+      <c r="AA57" s="26"/>
+      <c r="AB57" s="26"/>
+      <c r="AC57" s="26"/>
+      <c r="AD57" s="26"/>
+    </row>
+    <row r="58" spans="1:30" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="26" t="s">
         <v>125</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>133</v>
+        <v>51</v>
       </c>
       <c r="C58" s="27">
         <v>42160</v>
       </c>
       <c r="D58" s="26">
-        <f t="shared" si="4"/>
-        <v>9</v>
+        <f>SUM(F58:AD58)</f>
+        <v>8</v>
       </c>
       <c r="E58" s="28">
         <v>9</v>
       </c>
-      <c r="P58" s="26">
+      <c r="G58" s="26">
+        <v>7</v>
+      </c>
+      <c r="H58" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="C59" s="27">
+        <v>42160</v>
+      </c>
+      <c r="D59" s="26">
+        <f>SUM(F59:AD59)</f>
+        <v>4</v>
+      </c>
+      <c r="E59" s="28">
+        <v>3</v>
+      </c>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="26"/>
+      <c r="I59" s="26"/>
+      <c r="J59" s="26"/>
+      <c r="K59" s="26"/>
+      <c r="L59" s="26"/>
+      <c r="M59" s="26"/>
+      <c r="N59" s="26"/>
+      <c r="O59" s="26"/>
+      <c r="P59" s="26">
+        <v>2</v>
+      </c>
+      <c r="Q59" s="26">
+        <v>2</v>
+      </c>
+      <c r="R59" s="26"/>
+      <c r="S59" s="26"/>
+      <c r="T59" s="26"/>
+      <c r="U59" s="26"/>
+      <c r="V59" s="26"/>
+      <c r="W59" s="26"/>
+      <c r="X59" s="26"/>
+      <c r="Y59" s="26"/>
+      <c r="Z59" s="26"/>
+      <c r="AA59" s="26"/>
+      <c r="AB59" s="26"/>
+      <c r="AC59" s="26"/>
+      <c r="AD59" s="26"/>
+    </row>
+    <row r="60" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C60" s="27">
+        <v>42160</v>
+      </c>
+      <c r="D60" s="26">
+        <f>SUM(F60:AD60)</f>
+        <v>4</v>
+      </c>
+      <c r="E60" s="28">
+        <v>3</v>
+      </c>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26"/>
+      <c r="I60" s="26"/>
+      <c r="J60" s="26"/>
+      <c r="K60" s="26"/>
+      <c r="L60" s="26"/>
+      <c r="M60" s="26"/>
+      <c r="N60" s="26"/>
+      <c r="O60" s="26"/>
+      <c r="P60" s="26">
+        <v>2</v>
+      </c>
+      <c r="Q60" s="26">
+        <v>2</v>
+      </c>
+      <c r="R60" s="26"/>
+      <c r="S60" s="26"/>
+      <c r="T60" s="26"/>
+      <c r="U60" s="26"/>
+      <c r="V60" s="26"/>
+      <c r="W60" s="26"/>
+      <c r="X60" s="26"/>
+      <c r="Y60" s="26"/>
+      <c r="Z60" s="26"/>
+      <c r="AA60" s="26"/>
+      <c r="AB60" s="26"/>
+      <c r="AC60" s="26"/>
+      <c r="AD60" s="26"/>
+    </row>
+    <row r="61" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C61" s="27">
+        <v>42160</v>
+      </c>
+      <c r="D61" s="26">
+        <f>SUM(F61:AD61)</f>
+        <v>9</v>
+      </c>
+      <c r="E61" s="28">
+        <v>9</v>
+      </c>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
+      <c r="J61" s="26"/>
+      <c r="K61" s="26"/>
+      <c r="L61" s="26"/>
+      <c r="M61" s="26"/>
+      <c r="N61" s="26"/>
+      <c r="O61" s="26"/>
+      <c r="P61" s="26">
         <v>5</v>
       </c>
-      <c r="Q58" s="26">
+      <c r="Q61" s="26">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="17" t="s">
+      <c r="R61" s="26"/>
+      <c r="S61" s="26"/>
+      <c r="T61" s="26"/>
+      <c r="U61" s="26"/>
+      <c r="V61" s="26"/>
+      <c r="W61" s="26"/>
+      <c r="X61" s="26"/>
+      <c r="Y61" s="26"/>
+      <c r="Z61" s="26"/>
+      <c r="AA61" s="26"/>
+      <c r="AB61" s="26"/>
+      <c r="AC61" s="26"/>
+      <c r="AD61" s="26"/>
+    </row>
+    <row r="62" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="B59" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C59" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D59" s="17">
-        <f t="shared" si="4"/>
+      <c r="B62" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C62" s="21">
+        <v>42190</v>
+      </c>
+      <c r="D62" s="20">
+        <f>SUM(F62:AD62)</f>
+        <v>9</v>
+      </c>
+      <c r="E62" s="22">
+        <v>9</v>
+      </c>
+      <c r="F62" s="20"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="20"/>
+      <c r="K62" s="20"/>
+      <c r="L62" s="20"/>
+      <c r="M62" s="20"/>
+      <c r="N62" s="20"/>
+      <c r="O62" s="20"/>
+      <c r="P62" s="20"/>
+      <c r="Q62" s="20"/>
+      <c r="R62" s="20"/>
+      <c r="S62" s="20"/>
+      <c r="T62" s="20">
+        <v>9</v>
+      </c>
+      <c r="U62" s="20"/>
+      <c r="V62" s="20"/>
+      <c r="W62" s="20"/>
+      <c r="X62" s="20"/>
+      <c r="Y62" s="20"/>
+      <c r="Z62" s="20"/>
+      <c r="AA62" s="20"/>
+      <c r="AB62" s="20"/>
+      <c r="AC62" s="20"/>
+      <c r="AD62" s="20"/>
+    </row>
+    <row r="63" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C63" s="24">
+        <v>42209</v>
+      </c>
+      <c r="D63" s="23">
+        <f>SUM(F63:AD63)</f>
+        <v>9</v>
+      </c>
+      <c r="E63" s="25">
+        <v>10</v>
+      </c>
+      <c r="F63" s="23"/>
+      <c r="G63" s="23"/>
+      <c r="H63" s="23"/>
+      <c r="I63" s="23"/>
+      <c r="J63" s="23"/>
+      <c r="K63" s="23"/>
+      <c r="L63" s="23"/>
+      <c r="M63" s="23"/>
+      <c r="N63" s="23"/>
+      <c r="O63" s="23"/>
+      <c r="P63" s="23"/>
+      <c r="Q63" s="23">
+        <v>5</v>
+      </c>
+      <c r="R63" s="23"/>
+      <c r="S63" s="23"/>
+      <c r="T63" s="23"/>
+      <c r="U63" s="23">
+        <v>2</v>
+      </c>
+      <c r="V63" s="23"/>
+      <c r="W63" s="23"/>
+      <c r="X63" s="23">
+        <v>2</v>
+      </c>
+      <c r="Y63" s="23"/>
+      <c r="Z63" s="23"/>
+      <c r="AA63" s="23"/>
+      <c r="AB63" s="23"/>
+      <c r="AC63" s="23"/>
+      <c r="AD63" s="23"/>
+    </row>
+    <row r="64" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B64" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C64" s="24">
+        <v>42209</v>
+      </c>
+      <c r="D64" s="23">
+        <f>SUM(F64:AD64)</f>
+        <v>6</v>
+      </c>
+      <c r="E64" s="25">
+        <v>5</v>
+      </c>
+      <c r="F64" s="23"/>
+      <c r="G64" s="23"/>
+      <c r="H64" s="23"/>
+      <c r="I64" s="23"/>
+      <c r="J64" s="23"/>
+      <c r="K64" s="23"/>
+      <c r="L64" s="23"/>
+      <c r="M64" s="23"/>
+      <c r="N64" s="23"/>
+      <c r="O64" s="23"/>
+      <c r="P64" s="23"/>
+      <c r="Q64" s="23">
+        <v>2</v>
+      </c>
+      <c r="R64" s="23"/>
+      <c r="S64" s="23"/>
+      <c r="T64" s="23"/>
+      <c r="U64" s="23">
+        <v>2</v>
+      </c>
+      <c r="V64" s="23"/>
+      <c r="W64" s="23"/>
+      <c r="X64" s="23">
+        <v>2</v>
+      </c>
+      <c r="Y64" s="23"/>
+      <c r="Z64" s="23"/>
+      <c r="AA64" s="23"/>
+      <c r="AB64" s="23"/>
+      <c r="AC64" s="23"/>
+      <c r="AD64" s="23"/>
+    </row>
+    <row r="65" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C65" s="24">
+        <v>42209</v>
+      </c>
+      <c r="D65" s="23">
+        <f>SUM(F65:AD65)</f>
+        <v>9</v>
+      </c>
+      <c r="E65" s="25">
+        <v>10</v>
+      </c>
+      <c r="F65" s="23"/>
+      <c r="G65" s="23">
+        <v>1</v>
+      </c>
+      <c r="H65" s="23"/>
+      <c r="I65" s="23"/>
+      <c r="J65" s="23"/>
+      <c r="K65" s="23"/>
+      <c r="L65" s="23"/>
+      <c r="M65" s="23"/>
+      <c r="N65" s="23"/>
+      <c r="O65" s="23"/>
+      <c r="P65" s="23"/>
+      <c r="Q65" s="23"/>
+      <c r="R65" s="23"/>
+      <c r="S65" s="23">
+        <v>7</v>
+      </c>
+      <c r="T65" s="23">
+        <v>1</v>
+      </c>
+      <c r="U65" s="23"/>
+      <c r="V65" s="23"/>
+      <c r="W65" s="23"/>
+      <c r="X65" s="23"/>
+      <c r="Y65" s="23"/>
+      <c r="Z65" s="23"/>
+      <c r="AA65" s="23"/>
+      <c r="AB65" s="23"/>
+      <c r="AC65" s="23"/>
+      <c r="AD65" s="23"/>
+    </row>
+    <row r="66" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C66" s="24">
+        <v>42209</v>
+      </c>
+      <c r="D66" s="23">
+        <f>SUM(F66:AD66)</f>
+        <v>11</v>
+      </c>
+      <c r="E66" s="25">
+        <v>10</v>
+      </c>
+      <c r="F66" s="23"/>
+      <c r="G66" s="23">
+        <v>1</v>
+      </c>
+      <c r="H66" s="23"/>
+      <c r="I66" s="23"/>
+      <c r="J66" s="23"/>
+      <c r="K66" s="23"/>
+      <c r="L66" s="23"/>
+      <c r="M66" s="23"/>
+      <c r="N66" s="23"/>
+      <c r="O66" s="23"/>
+      <c r="P66" s="23"/>
+      <c r="Q66" s="23"/>
+      <c r="R66" s="23">
+        <v>2</v>
+      </c>
+      <c r="S66" s="23">
+        <v>5</v>
+      </c>
+      <c r="T66" s="23"/>
+      <c r="U66" s="23"/>
+      <c r="V66" s="23"/>
+      <c r="W66" s="23">
+        <v>3</v>
+      </c>
+      <c r="X66" s="23"/>
+      <c r="Y66" s="23"/>
+      <c r="Z66" s="23"/>
+      <c r="AA66" s="23"/>
+      <c r="AB66" s="23"/>
+      <c r="AC66" s="23"/>
+      <c r="AD66" s="23"/>
+    </row>
+    <row r="67" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" s="36">
+        <v>42223</v>
+      </c>
+      <c r="D67" s="35">
+        <f>SUM(F67:AD67)</f>
+        <v>5</v>
+      </c>
+      <c r="E67" s="37">
+        <v>5</v>
+      </c>
+      <c r="F67" s="35"/>
+      <c r="G67" s="35"/>
+      <c r="H67" s="35"/>
+      <c r="I67" s="35"/>
+      <c r="J67" s="35"/>
+      <c r="K67" s="35"/>
+      <c r="L67" s="35"/>
+      <c r="M67" s="35"/>
+      <c r="N67" s="35"/>
+      <c r="O67" s="35"/>
+      <c r="P67" s="35"/>
+      <c r="Q67" s="35"/>
+      <c r="R67" s="35"/>
+      <c r="S67" s="35"/>
+      <c r="T67" s="35"/>
+      <c r="U67" s="35"/>
+      <c r="V67" s="35"/>
+      <c r="W67" s="35">
+        <v>5</v>
+      </c>
+      <c r="X67" s="35"/>
+      <c r="Y67" s="35"/>
+      <c r="Z67" s="35"/>
+      <c r="AA67" s="35"/>
+      <c r="AB67" s="35"/>
+      <c r="AC67" s="35"/>
+      <c r="AD67" s="35"/>
+    </row>
+    <row r="68" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="C68" s="36">
+        <v>42223</v>
+      </c>
+      <c r="D68" s="35">
+        <f>SUM(F68:AD68)</f>
+        <v>2</v>
+      </c>
+      <c r="E68" s="37">
+        <v>9</v>
+      </c>
+      <c r="F68" s="35"/>
+      <c r="G68" s="35"/>
+      <c r="H68" s="35"/>
+      <c r="I68" s="35"/>
+      <c r="J68" s="35"/>
+      <c r="K68" s="35"/>
+      <c r="L68" s="35"/>
+      <c r="M68" s="35"/>
+      <c r="N68" s="35"/>
+      <c r="O68" s="35"/>
+      <c r="P68" s="35"/>
+      <c r="Q68" s="35"/>
+      <c r="R68" s="35"/>
+      <c r="S68" s="35"/>
+      <c r="T68" s="35"/>
+      <c r="U68" s="35"/>
+      <c r="V68" s="35"/>
+      <c r="W68" s="35">
+        <v>2</v>
+      </c>
+      <c r="X68" s="35"/>
+      <c r="Y68" s="35"/>
+      <c r="Z68" s="35"/>
+      <c r="AA68" s="35"/>
+      <c r="AB68" s="35"/>
+      <c r="AC68" s="35"/>
+      <c r="AD68" s="35"/>
+    </row>
+    <row r="69" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="C69" s="36">
+        <v>42223</v>
+      </c>
+      <c r="D69" s="35">
+        <f>SUM(F69:AD69)</f>
+        <v>5</v>
+      </c>
+      <c r="E69" s="37">
+        <v>5</v>
+      </c>
+      <c r="F69" s="35"/>
+      <c r="G69" s="35"/>
+      <c r="H69" s="35"/>
+      <c r="I69" s="35"/>
+      <c r="J69" s="35"/>
+      <c r="K69" s="35"/>
+      <c r="L69" s="35"/>
+      <c r="M69" s="35"/>
+      <c r="N69" s="35"/>
+      <c r="O69" s="35"/>
+      <c r="P69" s="35"/>
+      <c r="Q69" s="35"/>
+      <c r="R69" s="35"/>
+      <c r="S69" s="35"/>
+      <c r="T69" s="35">
+        <v>5</v>
+      </c>
+      <c r="U69" s="35"/>
+      <c r="V69" s="35"/>
+      <c r="W69" s="35"/>
+      <c r="X69" s="35"/>
+      <c r="Y69" s="35"/>
+      <c r="Z69" s="35"/>
+      <c r="AA69" s="35"/>
+      <c r="AB69" s="35"/>
+      <c r="AC69" s="35"/>
+      <c r="AD69" s="35"/>
+    </row>
+    <row r="70" spans="1:30" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C70" s="36">
+        <v>42223</v>
+      </c>
+      <c r="D70" s="35">
+        <f>SUM(F70:AD70)</f>
+        <v>5</v>
+      </c>
+      <c r="E70" s="37">
+        <v>4</v>
+      </c>
+      <c r="N70" s="35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="C71" s="36">
+        <v>42224</v>
+      </c>
+      <c r="D71" s="35">
+        <f>SUM(F71:AD71)</f>
         <v>0</v>
       </c>
-      <c r="E59" s="19">
+      <c r="E71" s="37">
+        <v>5</v>
+      </c>
+      <c r="F71" s="35"/>
+      <c r="G71" s="35"/>
+      <c r="H71" s="35"/>
+      <c r="I71" s="35"/>
+      <c r="J71" s="35"/>
+      <c r="K71" s="35"/>
+      <c r="L71" s="35"/>
+      <c r="M71" s="35"/>
+      <c r="N71" s="35"/>
+      <c r="O71" s="35"/>
+      <c r="P71" s="35"/>
+      <c r="Q71" s="35"/>
+      <c r="R71" s="35"/>
+      <c r="S71" s="35"/>
+      <c r="T71" s="35"/>
+      <c r="U71" s="35"/>
+      <c r="V71" s="35"/>
+      <c r="W71" s="35"/>
+      <c r="X71" s="35"/>
+      <c r="Y71" s="35"/>
+      <c r="Z71" s="35"/>
+      <c r="AA71" s="35"/>
+      <c r="AB71" s="35"/>
+      <c r="AC71" s="35"/>
+      <c r="AD71" s="35"/>
+    </row>
+    <row r="72" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="35" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="60" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="17" t="s">
+      <c r="B72" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="C72" s="36">
+        <v>42224</v>
+      </c>
+      <c r="D72" s="35">
+        <f>SUM(F72:AD72)</f>
+        <v>17</v>
+      </c>
+      <c r="E72" s="37">
+        <v>15</v>
+      </c>
+      <c r="F72" s="35"/>
+      <c r="G72" s="35"/>
+      <c r="H72" s="35"/>
+      <c r="I72" s="35"/>
+      <c r="J72" s="35"/>
+      <c r="K72" s="35"/>
+      <c r="L72" s="35"/>
+      <c r="M72" s="35"/>
+      <c r="N72" s="35"/>
+      <c r="O72" s="35"/>
+      <c r="P72" s="35"/>
+      <c r="Q72" s="35"/>
+      <c r="R72" s="35"/>
+      <c r="S72" s="35"/>
+      <c r="T72" s="35">
+        <v>1</v>
+      </c>
+      <c r="U72" s="35">
+        <v>7</v>
+      </c>
+      <c r="V72" s="35">
+        <v>3</v>
+      </c>
+      <c r="W72" s="35">
+        <v>6</v>
+      </c>
+      <c r="X72" s="35"/>
+      <c r="Y72" s="35"/>
+      <c r="Z72" s="35"/>
+      <c r="AA72" s="35"/>
+      <c r="AB72" s="35"/>
+      <c r="AC72" s="35"/>
+      <c r="AD72" s="35"/>
+    </row>
+    <row r="73" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" s="30">
+        <v>42230</v>
+      </c>
+      <c r="D73" s="29">
+        <f>SUM(F73:AD73)</f>
+        <v>7</v>
+      </c>
+      <c r="E73" s="31">
+        <v>7</v>
+      </c>
+      <c r="F73" s="29"/>
+      <c r="G73" s="29"/>
+      <c r="H73" s="29"/>
+      <c r="I73" s="29"/>
+      <c r="J73" s="29"/>
+      <c r="K73" s="29"/>
+      <c r="L73" s="29"/>
+      <c r="M73" s="29"/>
+      <c r="N73" s="29"/>
+      <c r="O73" s="29"/>
+      <c r="P73" s="29"/>
+      <c r="Q73" s="29"/>
+      <c r="R73" s="29"/>
+      <c r="S73" s="29"/>
+      <c r="T73" s="29">
+        <v>2</v>
+      </c>
+      <c r="U73" s="29">
+        <v>5</v>
+      </c>
+      <c r="V73" s="29"/>
+      <c r="W73" s="29"/>
+      <c r="X73" s="29"/>
+      <c r="Y73" s="29"/>
+      <c r="Z73" s="29"/>
+      <c r="AA73" s="29"/>
+      <c r="AB73" s="29"/>
+      <c r="AC73" s="29"/>
+      <c r="AD73" s="29"/>
+    </row>
+    <row r="74" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="C74" s="33">
+        <v>42237</v>
+      </c>
+      <c r="D74" s="32">
+        <f>SUM(F74:AD74)</f>
+        <v>7</v>
+      </c>
+      <c r="E74" s="34">
+        <v>6</v>
+      </c>
+      <c r="F74" s="32"/>
+      <c r="G74" s="32"/>
+      <c r="H74" s="32"/>
+      <c r="I74" s="32"/>
+      <c r="J74" s="32"/>
+      <c r="K74" s="32"/>
+      <c r="L74" s="32"/>
+      <c r="M74" s="32"/>
+      <c r="N74" s="32"/>
+      <c r="O74" s="32"/>
+      <c r="P74" s="32"/>
+      <c r="Q74" s="32"/>
+      <c r="R74" s="32"/>
+      <c r="S74" s="32"/>
+      <c r="T74" s="32">
+        <v>2</v>
+      </c>
+      <c r="U74" s="32">
+        <v>5</v>
+      </c>
+      <c r="V74" s="32"/>
+      <c r="W74" s="32"/>
+      <c r="X74" s="32"/>
+      <c r="Y74" s="32"/>
+      <c r="Z74" s="32"/>
+      <c r="AA74" s="32"/>
+      <c r="AB74" s="32"/>
+      <c r="AC74" s="32"/>
+      <c r="AD74" s="32"/>
+    </row>
+    <row r="75" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="C75" s="39">
+        <v>42251</v>
+      </c>
+      <c r="D75" s="38">
+        <f>SUM(F75:AD75)</f>
+        <v>0</v>
+      </c>
+      <c r="E75" s="40">
+        <v>15</v>
+      </c>
+      <c r="F75" s="38"/>
+      <c r="G75" s="38"/>
+      <c r="H75" s="38"/>
+      <c r="I75" s="38"/>
+      <c r="J75" s="38"/>
+      <c r="K75" s="38"/>
+      <c r="L75" s="38"/>
+      <c r="M75" s="38"/>
+      <c r="N75" s="38"/>
+      <c r="O75" s="38"/>
+      <c r="P75" s="38"/>
+      <c r="Q75" s="38"/>
+      <c r="R75" s="38"/>
+      <c r="S75" s="38"/>
+      <c r="T75" s="38"/>
+      <c r="U75" s="38"/>
+      <c r="V75" s="38"/>
+      <c r="W75" s="38"/>
+      <c r="X75" s="38"/>
+      <c r="Y75" s="38"/>
+      <c r="Z75" s="38"/>
+      <c r="AA75" s="38"/>
+      <c r="AB75" s="38"/>
+      <c r="AC75" s="38"/>
+      <c r="AD75" s="38"/>
+    </row>
+    <row r="76" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C76" s="39">
+        <v>42251</v>
+      </c>
+      <c r="D76" s="38">
+        <f>SUM(F76:AD76)</f>
+        <v>0</v>
+      </c>
+      <c r="E76" s="40">
+        <v>12</v>
+      </c>
+      <c r="F76" s="38"/>
+      <c r="G76" s="38"/>
+      <c r="H76" s="38"/>
+      <c r="I76" s="38"/>
+      <c r="J76" s="38"/>
+      <c r="K76" s="38"/>
+      <c r="L76" s="38"/>
+      <c r="M76" s="38"/>
+      <c r="N76" s="38"/>
+      <c r="O76" s="38"/>
+      <c r="P76" s="38"/>
+      <c r="Q76" s="38"/>
+      <c r="R76" s="38"/>
+      <c r="S76" s="38"/>
+      <c r="T76" s="38"/>
+      <c r="U76" s="38"/>
+      <c r="V76" s="38"/>
+      <c r="W76" s="38"/>
+      <c r="X76" s="38"/>
+      <c r="Y76" s="38"/>
+      <c r="Z76" s="38"/>
+      <c r="AA76" s="38"/>
+      <c r="AB76" s="38"/>
+      <c r="AC76" s="38"/>
+      <c r="AD76" s="38"/>
+    </row>
+    <row r="77" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="C77" s="39">
+        <v>42251</v>
+      </c>
+      <c r="D77" s="38">
+        <f>SUM(F77:AD77)</f>
+        <v>5</v>
+      </c>
+      <c r="E77" s="40">
+        <v>6</v>
+      </c>
+      <c r="F77" s="38"/>
+      <c r="G77" s="38"/>
+      <c r="H77" s="38"/>
+      <c r="I77" s="38"/>
+      <c r="J77" s="38"/>
+      <c r="K77" s="38"/>
+      <c r="L77" s="38"/>
+      <c r="M77" s="38"/>
+      <c r="N77" s="38"/>
+      <c r="O77" s="38"/>
+      <c r="P77" s="38"/>
+      <c r="Q77" s="38"/>
+      <c r="R77" s="38"/>
+      <c r="S77" s="38">
+        <v>5</v>
+      </c>
+      <c r="T77" s="38"/>
+      <c r="U77" s="38"/>
+      <c r="V77" s="38"/>
+      <c r="W77" s="38"/>
+      <c r="X77" s="38"/>
+      <c r="Y77" s="38"/>
+      <c r="Z77" s="38"/>
+      <c r="AA77" s="38"/>
+      <c r="AB77" s="38"/>
+      <c r="AC77" s="38"/>
+      <c r="AD77" s="38"/>
+    </row>
+    <row r="78" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="B60" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C60" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D60" s="17">
-        <f t="shared" si="4"/>
+      <c r="B78" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C78" s="39">
+        <v>42251</v>
+      </c>
+      <c r="D78" s="38">
+        <f>SUM(F78:AD78)</f>
+        <v>7</v>
+      </c>
+      <c r="E78" s="40">
+        <v>7</v>
+      </c>
+      <c r="F78" s="38"/>
+      <c r="G78" s="38"/>
+      <c r="H78" s="38"/>
+      <c r="I78" s="38"/>
+      <c r="J78" s="38"/>
+      <c r="K78" s="38"/>
+      <c r="L78" s="38"/>
+      <c r="M78" s="38"/>
+      <c r="N78" s="38"/>
+      <c r="O78" s="38"/>
+      <c r="P78" s="38"/>
+      <c r="Q78" s="38"/>
+      <c r="R78" s="38"/>
+      <c r="S78" s="38">
+        <v>7</v>
+      </c>
+      <c r="T78" s="38"/>
+      <c r="U78" s="38"/>
+      <c r="V78" s="38"/>
+      <c r="W78" s="38"/>
+      <c r="X78" s="38"/>
+      <c r="Y78" s="38"/>
+      <c r="Z78" s="38"/>
+      <c r="AA78" s="38"/>
+      <c r="AB78" s="38"/>
+      <c r="AC78" s="38"/>
+      <c r="AD78" s="38"/>
+    </row>
+    <row r="79" spans="1:30" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="B79" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C79" s="39">
+        <v>42251</v>
+      </c>
+      <c r="D79" s="38">
+        <f>SUM(F79:AD79)</f>
         <v>0</v>
       </c>
-      <c r="E60" s="19">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C61" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D61" s="17">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="E61" s="19">
-        <v>13</v>
-      </c>
-      <c r="F61" s="17">
-        <v>3</v>
-      </c>
-      <c r="G61" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B62" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="C62" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D62" s="17">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="E62" s="19">
-        <v>13</v>
-      </c>
-      <c r="F62" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B63" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C63" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D63" s="17">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="E63" s="19">
-        <v>8</v>
-      </c>
-      <c r="F63" s="17">
-        <v>3</v>
-      </c>
-      <c r="G63" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:20" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B64" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C64" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D64" s="17">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="E64" s="19">
-        <v>6</v>
-      </c>
-      <c r="F64" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B65" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="C65" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D65" s="17">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="E65" s="19">
-        <v>8</v>
-      </c>
-      <c r="F65" s="17">
-        <v>3</v>
-      </c>
-      <c r="G65" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C66" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D66" s="17">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="E66" s="19">
-        <v>8</v>
-      </c>
-      <c r="F66" s="17">
-        <v>3</v>
-      </c>
-      <c r="G66" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:29" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B67" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="C67" s="24">
-        <v>42209</v>
-      </c>
-      <c r="D67" s="23">
-        <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="E67" s="25">
-        <v>10</v>
-      </c>
-      <c r="G67" s="23">
-        <v>1</v>
-      </c>
-      <c r="R67" s="23">
-        <v>2</v>
-      </c>
-      <c r="S67" s="23">
+      <c r="E79" s="40">
         <v>5</v>
       </c>
-      <c r="W67" s="23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="C68" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D68" s="17">
-        <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="E68" s="19">
-        <v>12</v>
-      </c>
-      <c r="G68" s="17">
-        <v>1</v>
-      </c>
-      <c r="H68" s="17">
-        <v>2</v>
-      </c>
-      <c r="J68" s="17">
-        <v>7</v>
-      </c>
-      <c r="K68" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="C69" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D69" s="17">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="E69" s="19">
-        <v>11</v>
-      </c>
-      <c r="N69" s="17">
-        <v>8</v>
-      </c>
-      <c r="O69" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="B70" s="35" t="s">
-        <v>142</v>
-      </c>
-      <c r="C70" s="36">
-        <v>42224</v>
-      </c>
-      <c r="D70" s="35">
-        <f t="shared" si="4"/>
-        <v>17</v>
-      </c>
-      <c r="E70" s="37">
-        <v>15</v>
-      </c>
-      <c r="T70" s="35">
-        <v>1</v>
-      </c>
-      <c r="U70" s="35">
-        <v>7</v>
-      </c>
-      <c r="V70" s="35">
-        <v>3</v>
-      </c>
-      <c r="W70" s="35">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C71" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D71" s="17">
-        <f t="shared" ref="D71:D129" si="5">SUM(F71:AD71)</f>
-        <v>0</v>
-      </c>
-      <c r="E71" s="19">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="72" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="C72" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D72" s="17">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="E72" s="19">
-        <v>12</v>
-      </c>
-      <c r="F72" s="17">
-        <v>3</v>
-      </c>
-      <c r="G72" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="C73" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D73" s="17">
-        <f t="shared" si="5"/>
-        <v>23</v>
-      </c>
-      <c r="E73" s="19">
-        <v>15</v>
-      </c>
-      <c r="F73" s="17">
-        <v>7</v>
-      </c>
-      <c r="G73" s="17">
-        <v>7</v>
-      </c>
-      <c r="N73" s="17">
-        <v>7</v>
-      </c>
-      <c r="Q73" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B74" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="C74" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D74" s="17">
-        <f t="shared" si="5"/>
-        <v>19</v>
-      </c>
-      <c r="E74" s="19">
-        <v>20</v>
-      </c>
-      <c r="G74" s="17">
-        <v>3</v>
-      </c>
-      <c r="H74" s="17">
-        <v>2</v>
-      </c>
-      <c r="Q74" s="17">
-        <v>4</v>
-      </c>
-      <c r="R74" s="17">
-        <v>2</v>
-      </c>
-      <c r="U74" s="17">
-        <v>7</v>
-      </c>
-      <c r="X74" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C75" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D75" s="17">
-        <f t="shared" si="5"/>
-        <v>18</v>
-      </c>
-      <c r="E75" s="19">
-        <v>20</v>
-      </c>
-      <c r="G75" s="17">
-        <v>3</v>
-      </c>
-      <c r="H75" s="17">
-        <v>2</v>
-      </c>
-      <c r="Q75" s="17">
-        <v>5</v>
-      </c>
-      <c r="U75" s="17">
-        <v>7</v>
-      </c>
-      <c r="X75" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B76" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="C76" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D76" s="17">
-        <f t="shared" si="5"/>
-        <v>11</v>
-      </c>
-      <c r="E76" s="19">
-        <v>6</v>
-      </c>
-      <c r="H76" s="17">
-        <v>0</v>
-      </c>
-      <c r="Q76" s="17">
-        <v>1</v>
-      </c>
-      <c r="R76" s="17">
-        <v>4</v>
-      </c>
-      <c r="U76" s="17">
-        <v>2</v>
-      </c>
-      <c r="V76" s="17">
-        <v>3</v>
-      </c>
-      <c r="X76" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="C77" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D77" s="17">
-        <f t="shared" si="5"/>
-        <v>19</v>
-      </c>
-      <c r="E77" s="19">
-        <v>22</v>
-      </c>
-      <c r="G77" s="17">
-        <v>3</v>
-      </c>
-      <c r="H77" s="17">
-        <v>2</v>
-      </c>
-      <c r="Q77" s="17">
-        <v>6</v>
-      </c>
-      <c r="U77" s="17">
-        <v>7</v>
-      </c>
-      <c r="X77" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B78" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="C78" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D78" s="17">
-        <f t="shared" si="5"/>
-        <v>21</v>
-      </c>
-      <c r="E78" s="19">
-        <v>21</v>
-      </c>
-      <c r="G78" s="17">
-        <v>3</v>
-      </c>
-      <c r="H78" s="17">
-        <v>7</v>
-      </c>
-      <c r="Q78" s="17">
-        <v>3</v>
-      </c>
-      <c r="U78" s="17">
-        <v>7</v>
-      </c>
-      <c r="X78" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B79" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="C79" s="18">
-        <v>42136</v>
-      </c>
-      <c r="D79" s="17">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="E79" s="19">
-        <v>12</v>
-      </c>
-      <c r="H79" s="17">
-        <v>0</v>
-      </c>
-      <c r="R79" s="17">
-        <v>5</v>
-      </c>
-      <c r="U79" s="17">
-        <v>2</v>
-      </c>
-      <c r="V79" s="17">
-        <v>2</v>
-      </c>
-      <c r="X79" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F79" s="38"/>
+      <c r="G79" s="38"/>
+      <c r="H79" s="38"/>
+      <c r="I79" s="38"/>
+      <c r="J79" s="38"/>
+      <c r="K79" s="38"/>
+      <c r="L79" s="38"/>
+      <c r="M79" s="38"/>
+      <c r="N79" s="38"/>
+      <c r="O79" s="38"/>
+      <c r="P79" s="38"/>
+      <c r="Q79" s="38"/>
+      <c r="R79" s="38"/>
+      <c r="S79" s="38"/>
+      <c r="T79" s="38"/>
+      <c r="U79" s="38"/>
+      <c r="V79" s="38"/>
+      <c r="W79" s="38"/>
+      <c r="X79" s="38"/>
+      <c r="Y79" s="38"/>
+      <c r="Z79" s="38"/>
+      <c r="AA79" s="38"/>
+      <c r="AB79" s="38"/>
+      <c r="AC79" s="38"/>
+      <c r="AD79" s="38"/>
+    </row>
+    <row r="80" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E80" s="11"/>
       <c r="AC80" s="16"/>
     </row>
@@ -5980,6 +6917,9 @@
       <c r="AC105" s="16"/>
     </row>
   </sheetData>
+  <sortState ref="A7:AD79">
+    <sortCondition ref="C7:C79"/>
+  </sortState>
   <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>

</xml_diff>